<commit_message>
title fade case study
</commit_message>
<xml_diff>
--- a/data/residential-mobility/historical-descriptives/station-info.xlsx
+++ b/data/residential-mobility/historical-descriptives/station-info.xlsx
@@ -538,11 +538,14 @@
   </sheetPr>
   <dimension ref="A1:Z71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I32" activeCellId="0" sqref="I32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.97"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
historical mobility analysis and text
</commit_message>
<xml_diff>
--- a/data/residential-mobility/historical-descriptives/station-info.xlsx
+++ b/data/residential-mobility/historical-descriptives/station-info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="137">
   <si>
     <t xml:space="preserve">station_fid</t>
   </si>
@@ -55,6 +55,12 @@
     <t xml:space="preserve">City</t>
   </si>
   <si>
+    <t xml:space="preserve">year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decade</t>
+  </si>
+  <si>
     <t xml:space="preserve">45 Street SW</t>
   </si>
   <si>
@@ -73,6 +79,9 @@
     <t xml:space="preserve">Calgray</t>
   </si>
   <si>
+    <t xml:space="preserve">2010s</t>
+  </si>
+  <si>
     <t xml:space="preserve">69 Street SW</t>
   </si>
   <si>
@@ -85,12 +94,18 @@
     <t xml:space="preserve">9-Oct-01</t>
   </si>
   <si>
+    <t xml:space="preserve">2000s</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brentwood</t>
   </si>
   <si>
     <t xml:space="preserve">30-Aug-90</t>
   </si>
   <si>
+    <t xml:space="preserve">1990s</t>
+  </si>
+  <si>
     <t xml:space="preserve">Canyon Meadows</t>
   </si>
   <si>
@@ -100,6 +115,9 @@
     <t xml:space="preserve">15-Jun-09</t>
   </si>
   <si>
+    <t xml:space="preserve">2005s</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dalhousie</t>
   </si>
   <si>
@@ -205,7 +223,7 @@
     <t xml:space="preserve">6-Jun-15</t>
   </si>
   <si>
-    <t xml:space="preserve">Bloor-Lansdowne</t>
+    <t xml:space="preserve">Bradford</t>
   </si>
   <si>
     <t xml:space="preserve">Barrie</t>
@@ -214,9 +232,6 @@
     <t xml:space="preserve">26-Jan-05</t>
   </si>
   <si>
-    <t xml:space="preserve">Bradford</t>
-  </si>
-  <si>
     <t xml:space="preserve">Don Mills</t>
   </si>
   <si>
@@ -289,9 +304,6 @@
     <t xml:space="preserve">Ligne 2 - Orange, Saint-JÃ©rÃ´me</t>
   </si>
   <si>
-    <t xml:space="preserve">Subway, Commuter</t>
-  </si>
-  <si>
     <t xml:space="preserve">28-Apr-07</t>
   </si>
   <si>
@@ -340,12 +352,6 @@
     <t xml:space="preserve">Burquitlam</t>
   </si>
   <si>
-    <t xml:space="preserve">Coquitlam Central</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Millennium Line, West Coast Express</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gilmore</t>
   </si>
   <si>
@@ -382,7 +388,7 @@
     <t xml:space="preserve">Marine Drive</t>
   </si>
   <si>
-    <t xml:space="preserve">Moody Centre</t>
+    <t xml:space="preserve">Mission City</t>
   </si>
   <si>
     <t xml:space="preserve">Oakridge-41st Avenue</t>
@@ -422,12 +428,6 @@
   </si>
   <si>
     <t xml:space="preserve">VCC-Clark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waterfront</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canada Line, Expo Line, West Coast Express</t>
   </si>
   <si>
     <t xml:space="preserve">Yaletown-Roundhouse</t>
@@ -506,13 +506,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -536,66 +544,71 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z71"/>
+  <dimension ref="A1:Y71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G46" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L58" activeCellId="0" sqref="L58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.97"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -608,28 +621,34 @@
         <v>-114.1541947</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
+      <c r="H2" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>2009</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>2012</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -643,28 +662,34 @@
         <v>-114.1876094</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>14</v>
+      <c r="H3" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>2009</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>2012</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -678,28 +703,34 @@
         <v>-114.0745188</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>20</v>
+      <c r="H4" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>2001</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -713,28 +744,34 @@
         <v>-114.1318034</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>22</v>
+      <c r="H5" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>1988</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>1990</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -748,28 +785,34 @@
         <v>-114.0697921</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>20</v>
+      <c r="H6" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>2001</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -783,28 +826,34 @@
         <v>-114.2065522</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>25</v>
+      <c r="H7" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>2005</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>2009</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -818,28 +867,34 @@
         <v>-114.1605254</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>27</v>
+      <c r="H8" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>2001</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>2003</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,28 +908,34 @@
         <v>-114.0872437</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>14</v>
+      <c r="H9" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>2009</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>2012</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -888,28 +949,34 @@
         <v>-114.0730564</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>30</v>
+      <c r="H10" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>2004</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -923,28 +990,34 @@
         <v>-113.9679024</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>32</v>
+      <c r="H11" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>2009</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>2012</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -958,28 +1031,34 @@
         <v>-113.9756529</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G12" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>34</v>
+      <c r="H12" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>2007</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -993,28 +1072,34 @@
         <v>-113.9481535</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>32</v>
+      <c r="H13" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>2009</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>2012</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,28 +1113,34 @@
         <v>-114.1250072</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>14</v>
+      <c r="H14" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>2009</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>2012</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1063,28 +1154,34 @@
         <v>-114.0705658</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G15" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>30</v>
+      <c r="H15" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>2004</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1098,28 +1195,34 @@
         <v>-114.1690442</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>14</v>
+      <c r="H16" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>2009</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>2012</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1133,28 +1236,34 @@
         <v>-114.0690009</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>30</v>
+      <c r="H17" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>2004</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1168,28 +1277,34 @@
         <v>-114.0991346</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>14</v>
+      <c r="H18" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>2009</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>2012</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1203,28 +1318,34 @@
         <v>-114.2355599</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>42</v>
+      <c r="H19" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="I19" s="0" t="n">
         <v>2012</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>2014</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1238,28 +1359,34 @@
         <v>-114.1363619</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>14</v>
+      <c r="H20" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>2009</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>2012</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1273,28 +1400,34 @@
         <v>-113.9817427</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>34</v>
+      <c r="H21" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>2007</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1308,147 +1441,157 @@
         <v>-113.500684</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>47</v>
+      <c r="H22" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>2010</v>
       </c>
-      <c r="J22" s="2" t="s">
-        <v>48</v>
+      <c r="J22" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>82</v>
-      </c>
-      <c r="B23" s="0" t="n">
-        <v>53.56599022</v>
-      </c>
-      <c r="C23" s="0" t="n">
-        <v>-113.5058161</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I23" s="0" t="n">
-        <v>2010</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="H23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" s="4"/>
       <c r="K23" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="L23" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>138</v>
+        <v>82</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>43.76666345</v>
+        <v>53.56599022</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>-79.38775574</v>
+        <v>-113.5058161</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>52</v>
       </c>
       <c r="F24" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="H24" s="2" t="s">
+      <c r="I24" s="0" t="n">
+        <v>2010</v>
+      </c>
+      <c r="J24" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J24" s="0" t="s">
-        <v>15</v>
       </c>
       <c r="K24" s="0" t="s">
         <v>55</v>
       </c>
+      <c r="L24" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>43.76919381</v>
+        <v>43.76666345</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>-79.37665237</v>
+        <v>-79.38775574</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G25" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="H25" s="2" t="s">
-        <v>54</v>
+      <c r="H25" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>43.65902698</v>
+        <v>43.76919381</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>-79.45193473</v>
+        <v>-79.37665237</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>58</v>
@@ -1459,52 +1602,64 @@
       <c r="G26" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H26" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I26" s="0" t="n">
-        <v>2011</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>60</v>
+      <c r="I26" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="L26" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>43.65774279</v>
+        <v>43.65902698</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>-79.44514929</v>
+        <v>-79.45193473</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="G27" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J27" s="0" t="s">
-        <v>15</v>
+      <c r="H27" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>2011</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1518,28 +1673,34 @@
         <v>-79.55602626</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="G28" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>63</v>
+      <c r="H28" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <v>2005</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1553,28 +1714,34 @@
         <v>-79.346976</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G29" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="H29" s="2" t="s">
-        <v>54</v>
+      <c r="H29" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="L29" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1588,28 +1755,34 @@
         <v>-79.45564745</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="G30" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>67</v>
+      <c r="H30" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="L30" s="0" t="n">
+        <v>2004</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1623,28 +1796,34 @@
         <v>-79.39838311</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="G31" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>70</v>
+      <c r="H31" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="L31" s="0" t="n">
+        <v>2016</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1658,28 +1837,34 @@
         <v>-79.3681364</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G32" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>72</v>
+      <c r="H32" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="L32" s="0" t="n">
+        <v>1978</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1693,28 +1878,34 @@
         <v>-79.78892853</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="G33" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="H33" s="2" t="s">
-        <v>75</v>
+      <c r="H33" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="L33" s="0" t="n">
+        <v>2007</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1728,28 +1919,34 @@
         <v>-79.3014606</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="G34" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>78</v>
+      <c r="H34" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K34" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="L34" s="0" t="n">
+        <v>2005</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1763,179 +1960,189 @@
         <v>-79.82243206</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="G35" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="H35" s="2" t="s">
-        <v>81</v>
+      <c r="H35" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="L35" s="0" t="n">
+        <v>2005</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>346</v>
-      </c>
-      <c r="B36" s="0" t="n">
-        <v>43.83750289</v>
-      </c>
-      <c r="C36" s="0" t="n">
-        <v>-79.49810886</v>
-      </c>
-      <c r="D36" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="E36" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="E36" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="F36" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="G36" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J36" s="0" t="s">
-        <v>15</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="H36" s="4"/>
       <c r="K36" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="L36" s="0" t="n">
+        <v>2008</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>383</v>
+        <v>346</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>43.85093466</v>
+        <v>43.83750289</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>-79.31483304</v>
+        <v>-79.49810886</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="G37" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="H37" s="2" t="s">
-        <v>85</v>
+      <c r="H37" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K37" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="L37" s="0" t="n">
+        <v>2001</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>43.69915725</v>
+        <v>43.85093466</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>-79.5110739</v>
+        <v>-79.31483304</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="G38" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I38" s="0" t="n">
-        <v>2011</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>60</v>
+      <c r="H38" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="K38" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="L38" s="0" t="n">
+        <v>1991</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>485</v>
+        <v>393</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>45.560698</v>
+        <v>43.69915725</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>-73.709389</v>
+        <v>-79.5110739</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="G39" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>90</v>
+        <v>35</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="I39" s="0" t="n">
-        <v>2002</v>
-      </c>
-      <c r="J39" s="0" t="n">
-        <v>1998</v>
+        <v>2011</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="K39" s="0" t="s">
-        <v>91</v>
+        <v>61</v>
+      </c>
+      <c r="L39" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>45.558436</v>
+        <v>45.560698</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>-73.722459</v>
+        <v>-73.709389</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>92</v>
@@ -1944,13 +2151,13 @@
         <v>93</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G40" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="H40" s="2" t="s">
-        <v>90</v>
+      <c r="H40" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="I40" s="0" t="n">
         <v>2002</v>
@@ -1959,123 +2166,127 @@
         <v>1998</v>
       </c>
       <c r="K40" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
+      </c>
+      <c r="L40" s="0" t="n">
+        <v>2007</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>652</v>
+        <v>486</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>49.184448</v>
+        <v>45.558436</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>-123.136286</v>
+        <v>-73.722459</v>
       </c>
       <c r="D41" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="H41" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E41" s="0" t="s">
+      <c r="I41" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="J41" s="0" t="n">
+        <v>1998</v>
+      </c>
+      <c r="K41" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="F41" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="G41" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I41" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K41" s="0" t="s">
-        <v>98</v>
+      <c r="L41" s="0" t="n">
+        <v>2007</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
-        <v>656</v>
-      </c>
-      <c r="B42" s="0" t="n">
-        <v>49.266384</v>
-      </c>
-      <c r="C42" s="0" t="n">
-        <v>-123.001664</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>99</v>
+        <v>499</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="G42" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="I42" s="0" t="n">
-        <v>1999</v>
-      </c>
-      <c r="J42" s="0" t="n">
-        <v>1998</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="H42" s="4"/>
       <c r="K42" s="0" t="s">
-        <v>98</v>
+        <v>95</v>
+      </c>
+      <c r="L42" s="0" t="n">
+        <v>2007</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>49.195535</v>
+        <v>49.184448</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>-123.125904</v>
+        <v>-123.136286</v>
       </c>
       <c r="D43" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="K43" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="E43" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="F43" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="G43" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I43" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K43" s="0" t="s">
-        <v>98</v>
+      <c r="L43" s="0" t="n">
+        <v>2009</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>49.262731</v>
+        <v>49.266384</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>-123.114815</v>
+        <v>-123.001664</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>103</v>
@@ -2084,118 +2295,136 @@
         <v>104</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G44" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H44" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I44" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>97</v>
+      <c r="H44" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <v>1999</v>
+      </c>
+      <c r="J44" s="0" t="n">
+        <v>1998</v>
       </c>
       <c r="K44" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L44" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>49.261426</v>
+        <v>49.195535</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>-122.889868</v>
+        <v>-123.125904</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E45" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="H45" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F45" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="G45" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="H45" s="2" t="s">
+      <c r="I45" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I45" s="0" t="n">
-        <v>1999</v>
-      </c>
-      <c r="J45" s="0" t="n">
-        <v>1998</v>
-      </c>
       <c r="K45" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L45" s="0" t="n">
+        <v>2009</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>49.274829</v>
+        <v>49.262731</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>-122.800597</v>
+        <v>-123.114815</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="G46" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="H46" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I46" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J46" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I46" s="0" t="n">
-        <v>1999</v>
-      </c>
-      <c r="J46" s="0" t="n">
-        <v>1998</v>
-      </c>
       <c r="K46" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L46" s="0" t="n">
+        <v>2009</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <v>668</v>
+        <v>659</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>49.264956</v>
+        <v>49.261426</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>-123.013507</v>
+        <v>-122.889868</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G47" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H47" s="2" t="s">
-        <v>101</v>
+      <c r="H47" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="I47" s="0" t="n">
         <v>1999</v>
@@ -2204,33 +2433,39 @@
         <v>1998</v>
       </c>
       <c r="K47" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L47" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>49.264729</v>
+        <v>49.264956</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>-122.982137</v>
+        <v>-123.013507</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G48" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H48" s="2" t="s">
-        <v>101</v>
+      <c r="H48" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="I48" s="0" t="n">
         <v>1999</v>
@@ -2239,33 +2474,39 @@
         <v>1998</v>
       </c>
       <c r="K48" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L48" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>49.277299</v>
+        <v>49.264729</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>-122.828179</v>
+        <v>-122.982137</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G49" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H49" s="2" t="s">
-        <v>101</v>
+      <c r="H49" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="I49" s="0" t="n">
         <v>1999</v>
@@ -2274,199 +2515,235 @@
         <v>1998</v>
       </c>
       <c r="K49" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L49" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>49.248556</v>
+        <v>49.277299</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>-123.115027</v>
+        <v>-122.828179</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G50" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H50" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I50" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>97</v>
+      <c r="H50" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I50" s="0" t="n">
+        <v>1999</v>
+      </c>
+      <c r="J50" s="0" t="n">
+        <v>1998</v>
       </c>
       <c r="K50" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L50" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>49.285748</v>
+        <v>49.248556</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>-122.791638</v>
+        <v>-123.115027</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E51" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="H51" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F51" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="G51" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="H51" s="2" t="s">
+      <c r="I51" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J51" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I51" s="0" t="n">
-        <v>1999</v>
-      </c>
-      <c r="J51" s="0" t="n">
-        <v>1998</v>
-      </c>
       <c r="K51" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L51" s="0" t="n">
+        <v>2009</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>49.225737</v>
+        <v>49.285748</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>-123.116569</v>
+        <v>-122.791638</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G52" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H52" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I52" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>97</v>
+      <c r="H52" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <v>1999</v>
+      </c>
+      <c r="J52" s="0" t="n">
+        <v>1998</v>
       </c>
       <c r="K52" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L52" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>49.173716</v>
+        <v>49.225737</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>-123.136355</v>
+        <v>-123.116569</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G53" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H53" s="2" t="s">
-        <v>96</v>
+      <c r="H53" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>97</v>
+        <v>17</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="K53" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L53" s="0" t="n">
+        <v>2009</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>49.280416</v>
+        <v>49.173716</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>-122.79382</v>
+        <v>-123.136355</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E54" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="H54" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F54" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="G54" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="H54" s="2" t="s">
+      <c r="I54" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J54" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I54" s="0" t="n">
-        <v>1999</v>
-      </c>
-      <c r="J54" s="0" t="n">
-        <v>1998</v>
-      </c>
       <c r="K54" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L54" s="0" t="n">
+        <v>2009</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>49.21650196</v>
+        <v>49.280416</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>-122.6662188</v>
+        <v>-122.79382</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>59</v>
@@ -2474,209 +2751,229 @@
       <c r="G55" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H55" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I55" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J55" s="0" t="s">
-        <v>15</v>
+      <c r="H55" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I55" s="0" t="n">
+        <v>1999</v>
+      </c>
+      <c r="J55" s="0" t="n">
+        <v>1998</v>
       </c>
       <c r="K55" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L55" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>49.209785</v>
+        <v>49.21650196</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>-123.117073</v>
+        <v>-122.6662188</v>
       </c>
       <c r="D56" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E56" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="E56" s="0" t="s">
-        <v>95</v>
-      </c>
       <c r="F56" s="0" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="G56" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H56" s="2" t="s">
-        <v>96</v>
+      <c r="H56" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>97</v>
+        <v>17</v>
+      </c>
+      <c r="J56" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="K56" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L56" s="0" t="n">
+        <v>1995</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>49.27796</v>
+        <v>49.209785</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>-122.845608</v>
+        <v>-123.117073</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="G57" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H57" s="2" t="s">
+      <c r="H57" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I57" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J57" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I57" s="0" t="n">
-        <v>1999</v>
-      </c>
-      <c r="J57" s="0" t="n">
-        <v>1983</v>
-      </c>
       <c r="K57" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L57" s="0" t="n">
+        <v>2009</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
-        <v>694</v>
-      </c>
-      <c r="B58" s="0" t="n">
-        <v>49.232943</v>
-      </c>
-      <c r="C58" s="0" t="n">
-        <v>-123.116271</v>
+        <v>689</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="G58" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I58" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>97</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="H58" s="4"/>
+      <c r="J58" s="4"/>
       <c r="K58" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L58" s="0" t="n">
+        <v>2005</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>49.26338535</v>
+        <v>49.232943</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>-123.1250223</v>
+        <v>-123.116271</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G59" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="H59" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I59" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J59" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I59" s="0" t="n">
-        <v>1999</v>
-      </c>
-      <c r="J59" s="0" t="n">
-        <v>1983</v>
-      </c>
       <c r="K59" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L59" s="0" t="n">
+        <v>2009</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>49.26660971</v>
+        <v>49.26338535</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>-123.1154277</v>
+        <v>-123.1250223</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>124</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G60" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H60" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I60" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J60" s="2" t="s">
-        <v>97</v>
+      <c r="H60" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I60" s="0" t="n">
+        <v>1999</v>
+      </c>
+      <c r="J60" s="0" t="n">
+        <v>1983</v>
       </c>
       <c r="K60" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L60" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>49.225662</v>
+        <v>49.26660971</v>
       </c>
       <c r="C61" s="0" t="n">
-        <v>-122.687865</v>
+        <v>-123.1154277</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="F61" s="0" t="s">
         <v>59</v>
@@ -2684,218 +2981,254 @@
       <c r="G61" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H61" s="2" t="s">
-        <v>118</v>
+      <c r="H61" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J61" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="K61" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L61" s="0" t="n">
+        <v>2009</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>49.261497</v>
+        <v>49.225662</v>
       </c>
       <c r="C62" s="0" t="n">
-        <v>-122.773982</v>
+        <v>-122.687865</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="G62" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H62" s="2" t="s">
-        <v>118</v>
+      <c r="H62" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J62" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K62" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L62" s="0" t="n">
+        <v>1995</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>49.212335</v>
+        <v>49.261497</v>
       </c>
       <c r="C63" s="0" t="n">
-        <v>-122.606021</v>
+        <v>-122.773982</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="G63" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H63" s="2" t="s">
-        <v>118</v>
+      <c r="H63" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J63" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K63" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L63" s="0" t="n">
+        <v>1995</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>49.25893</v>
+        <v>49.212335</v>
       </c>
       <c r="C64" s="0" t="n">
-        <v>-123.045286</v>
+        <v>-122.606021</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="G64" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H64" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="I64" s="0" t="n">
-        <v>1999</v>
-      </c>
-      <c r="J64" s="0" t="n">
-        <v>1983</v>
+      <c r="H64" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I64" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J64" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="K64" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L64" s="0" t="n">
+        <v>1995</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>49.168295</v>
+        <v>49.25893</v>
       </c>
       <c r="C65" s="0" t="n">
-        <v>-123.136345</v>
+        <v>-123.045286</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G65" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H65" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I65" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J65" s="2" t="s">
-        <v>97</v>
+      <c r="H65" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I65" s="0" t="n">
+        <v>1999</v>
+      </c>
+      <c r="J65" s="0" t="n">
+        <v>1983</v>
       </c>
       <c r="K65" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L65" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>49.26076</v>
+        <v>49.168295</v>
       </c>
       <c r="C66" s="0" t="n">
-        <v>-123.032865</v>
+        <v>-123.136345</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E66" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G66" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="H66" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F66" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="G66" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="H66" s="2" t="s">
+      <c r="I66" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J66" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I66" s="0" t="n">
-        <v>1999</v>
-      </c>
-      <c r="J66" s="0" t="n">
-        <v>1983</v>
-      </c>
       <c r="K66" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L66" s="0" t="n">
+        <v>2009</v>
+      </c>
+      <c r="M66" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>49.259163</v>
+        <v>49.26076</v>
       </c>
       <c r="C67" s="0" t="n">
-        <v>-122.963858</v>
+        <v>-123.032865</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G67" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H67" s="2" t="s">
-        <v>101</v>
+      <c r="H67" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="I67" s="0" t="n">
         <v>1999</v>
@@ -2904,112 +3237,136 @@
         <v>1983</v>
       </c>
       <c r="K67" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L67" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="M67" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>49.282419</v>
+        <v>49.259163</v>
       </c>
       <c r="C68" s="0" t="n">
-        <v>-123.118192</v>
+        <v>-122.963858</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G68" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H68" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I68" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J68" s="2" t="s">
-        <v>97</v>
+      <c r="H68" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I68" s="0" t="n">
+        <v>1999</v>
+      </c>
+      <c r="J68" s="0" t="n">
+        <v>1983</v>
       </c>
       <c r="K68" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L68" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="M68" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>49.265767</v>
+        <v>49.282419</v>
       </c>
       <c r="C69" s="0" t="n">
-        <v>-123.078798</v>
+        <v>-123.118192</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E69" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G69" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="H69" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F69" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="G69" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="H69" s="2" t="s">
+      <c r="I69" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J69" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I69" s="0" t="n">
-        <v>1999</v>
-      </c>
-      <c r="J69" s="0" t="n">
-        <v>1983</v>
-      </c>
       <c r="K69" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L69" s="0" t="n">
+        <v>2009</v>
+      </c>
+      <c r="M69" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B70" s="0" t="n">
-        <v>49.28615001</v>
+        <v>49.265767</v>
       </c>
       <c r="C70" s="0" t="n">
-        <v>-123.1123</v>
+        <v>-123.078798</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>135</v>
+        <v>104</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="G70" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H70" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I70" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J70" s="2" t="s">
-        <v>97</v>
+      <c r="H70" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I70" s="0" t="n">
+        <v>1999</v>
+      </c>
+      <c r="J70" s="0" t="n">
+        <v>1983</v>
       </c>
       <c r="K70" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L70" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="M70" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3026,25 +3383,31 @@
         <v>136</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G71" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H71" s="2" t="s">
-        <v>96</v>
+      <c r="H71" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J71" s="2" t="s">
-        <v>97</v>
+        <v>17</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="K71" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="L71" s="0" t="n">
+        <v>2009</v>
+      </c>
+      <c r="M71" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>